<commit_message>
feat: add terms billing model property to product item
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-agreements-parameters-not-all-columns.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-agreements-parameters-not-all-columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavellonkin/Documents/git/swo-marketplace-cli/tests/product_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susana.vazquez/Projects/swo-marketplace-cli/tests/product_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B377938B-6DD8-B641-8D53-AEA8B71E76D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12407CFF-AC24-2844-916C-34BDB837F17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="124">
   <si>
     <t>General Information</t>
   </si>
@@ -306,9 +306,6 @@
     <t>ERP Item ID</t>
   </si>
   <si>
-    <t>Billing Frequency</t>
-  </si>
-  <si>
     <t>Commitment Term</t>
   </si>
   <si>
@@ -439,6 +436,18 @@
   </si>
   <si>
     <t>Termination order validation (draft)</t>
+  </si>
+  <si>
+    <t>Billing Model</t>
+  </si>
+  <si>
+    <t>Billing Period</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>usage</t>
   </si>
 </sst>
 </file>
@@ -517,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -540,9 +549,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,9 +569,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -599,7 +609,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -705,7 +715,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -847,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -989,92 +999,92 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
         <v>112</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1956,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1969,15 +1979,15 @@
     <col min="3" max="3" width="30.1640625" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="69.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="13" width="18.1640625" customWidth="1"/>
-    <col min="14" max="16" width="27.1640625" customWidth="1"/>
-    <col min="17" max="18" width="24.5" customWidth="1"/>
+    <col min="6" max="7" width="69.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="14" width="18.1640625" customWidth="1"/>
+    <col min="15" max="17" width="27.1640625" customWidth="1"/>
+    <col min="18" max="19" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1997,101 +2007,107 @@
         <v>25</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
         <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" t="s">
         <v>87</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>89</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
         <v>90</v>
       </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>91</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" s="4">
+        <v>45292</v>
+      </c>
+      <c r="S2" s="4">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>92</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>45292</v>
-      </c>
-      <c r="R2" s="4">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -2100,50 +2116,56 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
         <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
         <v>87</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
         <v>94</v>
       </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>95</v>
       </c>
-      <c r="P3" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>45292</v>
-      </c>
       <c r="R3" s="5">
         <v>45292</v>
       </c>
+      <c r="S3" s="5">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G4" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2191,7 +2213,7 @@
         <v>26</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>18</v>
@@ -2202,22 +2224,22 @@
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="4">
         <v>45292</v>
@@ -2228,22 +2250,22 @@
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="5">
         <v>45292</v>

</xml_diff>